<commit_message>
Exchange rate and water
</commit_message>
<xml_diff>
--- a/kenya_sut/Database/Shock_pulp.xlsx
+++ b/kenya_sut/Database/Shock_pulp.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\negar\Documents\GitHub\CIVICS_Kenya\kenya_sut\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gollinucci\Documents\GitHub\CIVICS_Kenya\kenya_sut\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A2194B-840D-404A-8E34-B3ABE5B498D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S" sheetId="7" r:id="rId1"/>
@@ -19,17 +20,25 @@
     <sheet name="Indeces" sheetId="8" r:id="rId5"/>
     <sheet name="main" sheetId="9" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="236">
   <si>
     <t>level_row</t>
   </si>
@@ -610,9 +619,6 @@
     <t>Increase in use of Petroleum weighted</t>
   </si>
   <si>
-    <t>Decrease in Unskilled labour weighted</t>
-  </si>
-  <si>
     <t>Decrease in Water Footprint weighted</t>
   </si>
   <si>
@@ -643,9 +649,6 @@
     <t>Hours of working of each machine</t>
   </si>
   <si>
-    <t>Num of machines</t>
-  </si>
-  <si>
     <t>hours</t>
   </si>
   <si>
@@ -676,9 +679,6 @@
     <t>kg/L</t>
   </si>
   <si>
-    <t xml:space="preserve">Decrease in Unskilled labour </t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -703,9 +703,6 @@
     <t>Z</t>
   </si>
   <si>
-    <t>WFN: Total water footprint (Mm3/yr) - Blue</t>
-  </si>
-  <si>
     <t>Aggregated</t>
   </si>
   <si>
@@ -722,12 +719,39 @@
   </si>
   <si>
     <t>0.107-0.112</t>
+  </si>
+  <si>
+    <t>Functional Unit</t>
+  </si>
+  <si>
+    <t>Productivity increase due to 100% new machines (not spoiling the cerry)</t>
+  </si>
+  <si>
+    <t>Maximum number of machines</t>
+  </si>
+  <si>
+    <t>Number of machines</t>
+  </si>
+  <si>
+    <t>Useful life of the pulping machines</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>Increase in Capital (agriculture) weighted</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>WFN: Total water footprint (Mm3/yr) - Green</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -901,7 +925,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -933,9 +957,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -964,6 +985,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1278,23 +1314,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.15625" style="1"/>
-    <col min="2" max="2" width="22.15625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="35.26171875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="22.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.15625" style="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1308,12 +1344,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="C2" t="s">
         <v>92</v>
@@ -1321,26 +1357,26 @@
       <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2">
-        <f>main!C26</f>
-        <v>-7.0957409331033561E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E2" s="38">
+        <f>main!C29</f>
+        <v>-4.2499999999999998E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Percentage, Absolute"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1349,22 +1385,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.15625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
     <col min="2" max="2" width="33" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.15625" style="1"/>
+    <col min="4" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1372,7 +1408,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1380,11 +1416,11 @@
         <v>67</v>
       </c>
       <c r="C2" s="1">
-        <f>main!C21</f>
-        <v>310</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <f>main!C24</f>
+        <v>0.155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1392,20 +1428,20 @@
         <v>75</v>
       </c>
       <c r="C3" s="1">
-        <f>main!C22</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <f>main!C25</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
     </row>
   </sheetData>
@@ -1413,7 +1449,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Indeces!$A$2:$A$72</xm:f>
           </x14:formula1>
@@ -1426,27 +1462,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.15625" style="1"/>
-    <col min="2" max="2" width="12.83984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.26171875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.26171875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.15625" style="1"/>
-    <col min="8" max="8" width="10.05078125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.15625" style="1"/>
+    <col min="7" max="7" width="9.109375" style="1"/>
+    <col min="8" max="8" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1466,10 +1502,10 @@
         <v>8</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1489,14 +1525,14 @@
         <v>7</v>
       </c>
       <c r="G2" s="5">
-        <f>-main!C23</f>
-        <v>-0.02</v>
+        <f>-main!C26</f>
+        <v>-1.0000000000000001E-5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1513,40 +1549,40 @@
         <v>92</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="G3" s="5">
+        <f>main!C27</f>
+        <v>1.0019056666666668E-2</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="G3" s="5">
-        <f>main!C24</f>
-        <v>2.1841543533333332</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="2"/>
       <c r="D6" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D6 B4:B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D6 B4:B6" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"commodity,activities"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"Percentage, Absolute"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3 B2:B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3 B2:B3" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>"Commodities,Activities"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1555,13 +1591,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000003000000}">
           <x14:formula1>
             <xm:f>Indeces!$A$2:$A$72</xm:f>
           </x14:formula1>
           <xm:sqref>C3 E2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000004000000}">
           <x14:formula1>
             <xm:f>Indeces!$B$2:$B$55</xm:f>
           </x14:formula1>
@@ -1574,24 +1610,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.15625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
     <col min="2" max="2" width="29" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.26171875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.15625" style="1"/>
+    <col min="6" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1608,15 +1644,15 @@
         <v>9</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>10</v>
+        <v>166</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>14</v>
@@ -1625,34 +1661,34 @@
         <v>92</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>7</v>
+        <v>219</v>
       </c>
       <c r="F2" s="2">
-        <f>main!C25</f>
-        <v>-5.0087583057200165E-3</v>
+        <f>main!C28</f>
+        <v>1.55E-2</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Commodities,Activities"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"Percentage, Absolute"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1660,13 +1696,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000002000000}">
           <x14:formula1>
             <xm:f>Indeces!$C$2:$C$37</xm:f>
           </x14:formula1>
           <xm:sqref>B2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000003000000}">
           <x14:formula1>
             <xm:f>Indeces!$B$2:$B$55</xm:f>
           </x14:formula1>
@@ -1679,21 +1715,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="56.83984375" customWidth="1"/>
-    <col min="3" max="3" width="47.15625" customWidth="1"/>
+    <col min="2" max="2" width="56.88671875" customWidth="1"/>
+    <col min="3" max="3" width="47.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>13</v>
       </c>
@@ -1705,7 +1741,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1716,7 +1752,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1727,7 +1763,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1738,7 +1774,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1749,7 +1785,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1760,7 +1796,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1771,7 +1807,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1782,7 +1818,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1793,7 +1829,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1804,7 +1840,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1815,7 +1851,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1826,7 +1862,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1837,7 +1873,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1848,7 +1884,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1859,7 +1895,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1870,7 +1906,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1881,7 +1917,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1892,7 +1928,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1903,7 +1939,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1914,7 +1950,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1925,7 +1961,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1936,7 +1972,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -1947,7 +1983,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1958,7 +1994,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1969,7 +2005,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -1980,7 +2016,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -1991,7 +2027,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -2002,7 +2038,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -2013,7 +2049,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -2024,7 +2060,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -2035,7 +2071,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -2046,7 +2082,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -2057,7 +2093,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -2068,7 +2104,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -2079,7 +2115,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -2090,7 +2126,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -2101,7 +2137,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -2109,7 +2145,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -2117,7 +2153,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>51</v>
       </c>
@@ -2125,7 +2161,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -2133,7 +2169,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>53</v>
       </c>
@@ -2141,7 +2177,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -2149,7 +2185,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -2157,7 +2193,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>56</v>
       </c>
@@ -2165,7 +2201,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>57</v>
       </c>
@@ -2173,7 +2209,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -2181,7 +2217,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -2189,7 +2225,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>60</v>
       </c>
@@ -2197,7 +2233,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>61</v>
       </c>
@@ -2205,7 +2241,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -2213,7 +2249,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -2221,7 +2257,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>64</v>
       </c>
@@ -2229,7 +2265,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>65</v>
       </c>
@@ -2237,7 +2273,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>66</v>
       </c>
@@ -2245,87 +2281,87 @@
         <v>135</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>83</v>
       </c>
@@ -2336,24 +2372,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.68359375" style="11" customWidth="1"/>
-    <col min="2" max="2" width="81.62890625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="10.20703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7890625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7890625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="57.15625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="81.6640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="15" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:7" s="15" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>174</v>
       </c>
@@ -2364,7 +2401,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>176</v>
@@ -2376,404 +2413,459 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="29" t="s">
         <v>172</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="24">
         <v>155</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25" t="s">
+      <c r="D2" s="24"/>
+      <c r="E2" s="24" t="s">
         <v>187</v>
       </c>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="31"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="30"/>
       <c r="B3" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="24">
         <v>5</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="24" t="s">
         <v>187</v>
       </c>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="31"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="30"/>
       <c r="B4" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="24">
         <v>400</v>
       </c>
-      <c r="D4" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="E4" s="25"/>
+      <c r="D4" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="E4" s="24"/>
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="31"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="30"/>
       <c r="B5" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="24">
         <v>800000</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
       <c r="F5" s="18"/>
       <c r="G5" s="18" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="31"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="30"/>
       <c r="B6" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="24">
         <v>8.3479305095333606E-2</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="31"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="30"/>
       <c r="B7" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="C7" s="24">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24" t="s">
         <v>195</v>
-      </c>
-      <c r="C7" s="25">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25" t="s">
-        <v>196</v>
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="31"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="30"/>
       <c r="B8" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="C8" s="25">
+        <v>198</v>
+      </c>
+      <c r="C8" s="24">
         <v>42.037999999999997</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25" t="s">
-        <v>198</v>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24" t="s">
+        <v>197</v>
       </c>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="31"/>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="30"/>
       <c r="B9" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="C9" s="25">
+        <v>201</v>
+      </c>
+      <c r="C9" s="24">
         <v>0.65</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="31"/>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="30"/>
       <c r="B10" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="C10" s="25">
+        <v>200</v>
+      </c>
+      <c r="C10" s="24">
         <v>0.5</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25" t="s">
-        <v>200</v>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24" t="s">
+        <v>199</v>
       </c>
       <c r="F10" s="18"/>
       <c r="G10" s="18"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="31"/>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="30"/>
       <c r="B11" s="17" t="s">
-        <v>209</v>
-      </c>
-      <c r="C11" s="25">
+        <v>207</v>
+      </c>
+      <c r="C11" s="24">
         <v>45</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25" t="s">
-        <v>210</v>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24" t="s">
+        <v>208</v>
       </c>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="31"/>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="30"/>
       <c r="B12" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="C12" s="25">
+        <v>209</v>
+      </c>
+      <c r="C12" s="24">
         <v>0.8</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25" t="s">
-        <v>214</v>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24" t="s">
+        <v>212</v>
       </c>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="31"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="30"/>
       <c r="B13" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="C13" s="25">
+        <v>210</v>
+      </c>
+      <c r="C13" s="24">
         <v>0.109</v>
       </c>
-      <c r="D13" s="25" t="s">
-        <v>230</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>213</v>
+      <c r="D13" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>211</v>
       </c>
       <c r="F13" s="18"/>
       <c r="G13" s="18"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="31"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="30"/>
       <c r="B14" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="C14" s="25">
+      <c r="C14" s="24">
         <v>-0.85</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="31"/>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="30"/>
       <c r="B15" s="17" t="s">
-        <v>215</v>
-      </c>
-      <c r="C15" s="25">
-        <v>-0.06</v>
-      </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
+        <v>231</v>
+      </c>
+      <c r="C15" s="24">
+        <v>10</v>
+      </c>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24" t="s">
+        <v>232</v>
+      </c>
       <c r="F15" s="18"/>
       <c r="G15" s="18"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="19" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="30"/>
+      <c r="B16" s="35" t="s">
+        <v>230</v>
+      </c>
+      <c r="C16" s="24">
+        <v>1</v>
+      </c>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="C16" s="26">
+      <c r="B17" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="C17" s="25">
         <v>0.3</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="32" t="s">
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="33"/>
+      <c r="B18" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="C18" s="25">
+        <v>0.02</v>
+      </c>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="31" t="s">
         <v>181</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B19" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="C19" s="27">
+        <f>C8*1000*C9/C20/C10</f>
+        <v>27.3247</v>
+      </c>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27" t="s">
         <v>203</v>
       </c>
-      <c r="C17" s="28">
-        <f>C8*1000*C9/C18/C10</f>
-        <v>27.3247</v>
-      </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28" t="s">
-        <v>205</v>
-      </c>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="32"/>
-      <c r="B18" s="23" t="s">
-        <v>204</v>
-      </c>
-      <c r="C18" s="28">
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="31"/>
+      <c r="B20" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="C20" s="27">
         <f>C5/C4</f>
         <v>2000</v>
       </c>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="32"/>
-      <c r="B19" s="23" t="s">
-        <v>206</v>
-      </c>
-      <c r="C19" s="28">
-        <f>C17*C7/C16</f>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="31"/>
+      <c r="B21" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="C21" s="27">
+        <f>C18*C16/C20</f>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="31"/>
+      <c r="B22" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="C22" s="37">
+        <f>C19*C7/C17</f>
         <v>100.19056666666668</v>
-      </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28" t="s">
-        <v>207</v>
-      </c>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="32"/>
-      <c r="B20" s="23" t="s">
-        <v>208</v>
-      </c>
-      <c r="C20" s="28">
-        <f>C19*3600/1000*C18/C11/C12*C13</f>
-        <v>2184.1543533333333</v>
-      </c>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28" t="s">
-        <v>187</v>
-      </c>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="29" t="s">
-        <v>182</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="C21" s="27">
-        <f>C18*C2/1000</f>
-        <v>310</v>
-      </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27" t="s">
-        <v>219</v>
-      </c>
-      <c r="F21" s="21" t="s">
-        <v>216</v>
-      </c>
-      <c r="G21" s="21"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="29"/>
-      <c r="B22" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="C22" s="27">
-        <f>C18*C3/1000</f>
-        <v>10</v>
       </c>
       <c r="D22" s="27"/>
       <c r="E22" s="27" t="s">
-        <v>219</v>
-      </c>
-      <c r="F22" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="31"/>
+      <c r="B23" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="C23" s="37">
+        <f>C22*3600/1000*C16/C11/C12</f>
+        <v>10.019056666666668</v>
+      </c>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="C24" s="26">
+        <f>C16*C2/1000</f>
+        <v>0.155</v>
+      </c>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26" t="s">
         <v>216</v>
       </c>
-      <c r="G22" s="21"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="29"/>
-      <c r="B23" s="20" t="s">
+      <c r="F24" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="G24" s="20"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="28"/>
+      <c r="B25" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="C25" s="26">
+        <f>C16*C3/1000</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="G25" s="20"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="28"/>
+      <c r="B26" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="C23" s="27">
-        <v>0.02</v>
-      </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="G23" s="21"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="29"/>
-      <c r="B24" s="20" t="s">
+      <c r="C26" s="26">
+        <f>C21</f>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="G26" s="20"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="28"/>
+      <c r="B27" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="C24" s="27">
-        <f>C20/1000</f>
-        <v>2.1841543533333332</v>
-      </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27" t="s">
-        <v>219</v>
-      </c>
-      <c r="F24" s="21" t="s">
-        <v>220</v>
-      </c>
-      <c r="G24" s="21"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="29"/>
-      <c r="B25" s="20" t="s">
+      <c r="C27" s="36">
+        <f>C23/1000</f>
+        <v>1.0019056666666668E-2</v>
+      </c>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="G27" s="20"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="28"/>
+      <c r="B28" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="C28" s="36">
+        <f>C24/C15</f>
+        <v>1.55E-2</v>
+      </c>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="G28" s="20"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="28"/>
+      <c r="B29" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="C25" s="27">
-        <f>C15*C6</f>
-        <v>-5.0087583057200165E-3</v>
-      </c>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="21" t="s">
-        <v>217</v>
-      </c>
-      <c r="G25" s="21"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="29"/>
-      <c r="B26" s="20" t="s">
-        <v>194</v>
-      </c>
-      <c r="C26" s="27">
-        <f>C14*C6</f>
-        <v>-7.0957409331033561E-2</v>
-      </c>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="21" t="s">
+      <c r="C29" s="36">
+        <f>C14*C16/C20</f>
+        <v>-4.2499999999999998E-4</v>
+      </c>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="F29" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="G29" s="20"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B32" s="32" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="G26" s="21"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B30" s="10" t="s">
-        <v>221</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="A2:A15"/>
-    <mergeCell ref="A17:A20"/>
+  <mergeCells count="4">
+    <mergeCell ref="A24:A29"/>
+    <mergeCell ref="A2:A16"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="A17:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Preparation for presentation of pulp mach shock
I've selected the only relevant categories for CO2.
Printed out some results.
</commit_message>
<xml_diff>
--- a/kenya_sut/Database/Shock_pulp.xlsx
+++ b/kenya_sut/Database/Shock_pulp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gollinucci\Documents\GitHub\CIVICS_Kenya\kenya_sut\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A2194B-840D-404A-8E34-B3ABE5B498D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3693E29F-8406-4705-B799-CAAF1DD77A03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -974,6 +974,18 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -986,20 +998,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1357,9 +1357,9 @@
       <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="38">
+      <c r="E2" s="33">
         <f>main!C29</f>
-        <v>-4.2499999999999998E-4</v>
+        <v>-0.85</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1417,7 +1417,7 @@
       </c>
       <c r="C2" s="1">
         <f>main!C24</f>
-        <v>0.155</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1429,7 +1429,7 @@
       </c>
       <c r="C3" s="1">
         <f>main!C25</f>
-        <v>5.0000000000000001E-3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1526,7 +1526,7 @@
       </c>
       <c r="G2" s="5">
         <f>-main!C26</f>
-        <v>-1.0000000000000001E-5</v>
+        <v>-0.02</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>222</v>
@@ -1553,7 +1553,7 @@
       </c>
       <c r="G3" s="5">
         <f>main!C27</f>
-        <v>1.0019056666666668E-2</v>
+        <v>20.038113333333335</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>222</v>
@@ -1665,7 +1665,7 @@
       </c>
       <c r="F2" s="2">
         <f>main!C28</f>
-        <v>1.55E-2</v>
+        <v>31</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>222</v>
@@ -2376,7 +2376,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2414,7 +2414,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="35" t="s">
         <v>172</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -2431,7 +2431,7 @@
       <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="30"/>
+      <c r="A3" s="36"/>
       <c r="B3" s="17" t="s">
         <v>173</v>
       </c>
@@ -2446,7 +2446,7 @@
       <c r="G3" s="18"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="30"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="17" t="s">
         <v>188</v>
       </c>
@@ -2461,7 +2461,7 @@
       <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="30"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="17" t="s">
         <v>189</v>
       </c>
@@ -2476,7 +2476,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="30"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="17" t="s">
         <v>191</v>
       </c>
@@ -2489,7 +2489,7 @@
       <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="30"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="17" t="s">
         <v>194</v>
       </c>
@@ -2504,7 +2504,7 @@
       <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="30"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="17" t="s">
         <v>198</v>
       </c>
@@ -2519,7 +2519,7 @@
       <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="30"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="17" t="s">
         <v>201</v>
       </c>
@@ -2532,7 +2532,7 @@
       <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="30"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="17" t="s">
         <v>200</v>
       </c>
@@ -2547,7 +2547,7 @@
       <c r="G10" s="18"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="30"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="17" t="s">
         <v>207</v>
       </c>
@@ -2562,7 +2562,7 @@
       <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="30"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="17" t="s">
         <v>209</v>
       </c>
@@ -2577,7 +2577,7 @@
       <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="30"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="17" t="s">
         <v>210</v>
       </c>
@@ -2594,7 +2594,7 @@
       <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="30"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="17" t="s">
         <v>186</v>
       </c>
@@ -2607,7 +2607,7 @@
       <c r="G14" s="18"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="30"/>
+      <c r="A15" s="36"/>
       <c r="B15" s="17" t="s">
         <v>231</v>
       </c>
@@ -2622,12 +2622,12 @@
       <c r="G15" s="18"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="30"/>
-      <c r="B16" s="35" t="s">
+      <c r="A16" s="36"/>
+      <c r="B16" s="30" t="s">
         <v>230</v>
       </c>
       <c r="C16" s="24">
-        <v>1</v>
+        <v>2000</v>
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="24"/>
@@ -2635,7 +2635,7 @@
       <c r="G16" s="18"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="38" t="s">
         <v>180</v>
       </c>
       <c r="B17" s="16" t="s">
@@ -2650,7 +2650,7 @@
       <c r="G17" s="21"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="33"/>
+      <c r="A18" s="38"/>
       <c r="B18" s="16" t="s">
         <v>228</v>
       </c>
@@ -2663,7 +2663,7 @@
       <c r="G18" s="21"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="37" t="s">
         <v>181</v>
       </c>
       <c r="B19" s="22" t="s">
@@ -2681,8 +2681,8 @@
       <c r="G19" s="23"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="31"/>
-      <c r="B20" s="34" t="s">
+      <c r="A20" s="37"/>
+      <c r="B20" s="29" t="s">
         <v>229</v>
       </c>
       <c r="C20" s="27">
@@ -2695,13 +2695,13 @@
       <c r="G20" s="23"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="31"/>
-      <c r="B21" s="34" t="s">
+      <c r="A21" s="37"/>
+      <c r="B21" s="29" t="s">
         <v>185</v>
       </c>
       <c r="C21" s="27">
         <f>C18*C16/C20</f>
-        <v>1.0000000000000001E-5</v>
+        <v>0.02</v>
       </c>
       <c r="D21" s="27"/>
       <c r="E21" s="27"/>
@@ -2709,11 +2709,11 @@
       <c r="G21" s="23"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="31"/>
+      <c r="A22" s="37"/>
       <c r="B22" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="C22" s="37">
+      <c r="C22" s="32">
         <f>C19*C7/C17</f>
         <v>100.19056666666668</v>
       </c>
@@ -2725,13 +2725,13 @@
       <c r="G22" s="23"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="31"/>
+      <c r="A23" s="37"/>
       <c r="B23" s="22" t="s">
         <v>206</v>
       </c>
-      <c r="C23" s="37">
+      <c r="C23" s="32">
         <f>C22*3600/1000*C16/C11/C12</f>
-        <v>10.019056666666668</v>
+        <v>20038.113333333335</v>
       </c>
       <c r="D23" s="27"/>
       <c r="E23" s="27" t="s">
@@ -2741,7 +2741,7 @@
       <c r="G23" s="23"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="34" t="s">
         <v>182</v>
       </c>
       <c r="B24" s="19" t="s">
@@ -2749,7 +2749,7 @@
       </c>
       <c r="C24" s="26">
         <f>C16*C2/1000</f>
-        <v>0.155</v>
+        <v>310</v>
       </c>
       <c r="D24" s="26"/>
       <c r="E24" s="26" t="s">
@@ -2761,13 +2761,13 @@
       <c r="G24" s="20"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="28"/>
+      <c r="A25" s="34"/>
       <c r="B25" s="19" t="s">
         <v>184</v>
       </c>
       <c r="C25" s="26">
         <f>C16*C3/1000</f>
-        <v>5.0000000000000001E-3</v>
+        <v>10</v>
       </c>
       <c r="D25" s="26"/>
       <c r="E25" s="26" t="s">
@@ -2779,13 +2779,13 @@
       <c r="G25" s="20"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="28"/>
+      <c r="A26" s="34"/>
       <c r="B26" s="19" t="s">
         <v>185</v>
       </c>
       <c r="C26" s="26">
         <f>C21</f>
-        <v>1.0000000000000001E-5</v>
+        <v>0.02</v>
       </c>
       <c r="D26" s="26"/>
       <c r="E26" s="26" t="s">
@@ -2797,13 +2797,13 @@
       <c r="G26" s="20"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="28"/>
+      <c r="A27" s="34"/>
       <c r="B27" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="C27" s="36">
+      <c r="C27" s="31">
         <f>C23/1000</f>
-        <v>1.0019056666666668E-2</v>
+        <v>20.038113333333335</v>
       </c>
       <c r="D27" s="26"/>
       <c r="E27" s="26" t="s">
@@ -2815,13 +2815,13 @@
       <c r="G27" s="20"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="28"/>
+      <c r="A28" s="34"/>
       <c r="B28" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="C28" s="36">
+      <c r="C28" s="31">
         <f>C24/C15</f>
-        <v>1.55E-2</v>
+        <v>31</v>
       </c>
       <c r="D28" s="26"/>
       <c r="E28" s="26" t="s">
@@ -2833,13 +2833,13 @@
       <c r="G28" s="20"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="28"/>
+      <c r="A29" s="34"/>
       <c r="B29" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="C29" s="36">
+      <c r="C29" s="31">
         <f>C14*C16/C20</f>
-        <v>-4.2499999999999998E-4</v>
+        <v>-0.85</v>
       </c>
       <c r="D29" s="26"/>
       <c r="E29" s="26" t="s">
@@ -2851,7 +2851,7 @@
       <c r="G29" s="20"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="28" t="s">
         <v>227</v>
       </c>
     </row>

</xml_diff>